<commit_message>
Convert shared Compound entities to XREFs with IDs.
- DICOM
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/DICOM_MODEL.xlsx
+++ b/molgenis-model-registry/src/test/resources/DICOM_MODEL.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1140" windowWidth="25600" windowHeight="16000" tabRatio="951"/>
+    <workbookView xWindow="6620" yWindow="920" windowWidth="26020" windowHeight="16680" tabRatio="951" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="25" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="tags" sheetId="26" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">attributes!$A$1:$J$378</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">attributes!$A$1:$J$381</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="844">
   <si>
     <t>description</t>
   </si>
@@ -2693,7 +2693,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="697">
+  <cellStyleXfs count="701">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3338,6 +3338,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3397,7 +3401,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="697">
+  <cellStyles count="701">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3874,6 +3878,8 @@
     <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4094,6 +4100,8 @@
     <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4425,7 +4433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -5041,11 +5049,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J378"/>
+  <dimension ref="A1:J381"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G319" sqref="G319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8104,7 +8112,7 @@
         <v>160</v>
       </c>
       <c r="D172" t="s">
-        <v>495</v>
+        <v>532</v>
       </c>
       <c r="E172" t="s">
         <v>160</v>
@@ -8363,7 +8371,7 @@
         <v>794</v>
       </c>
       <c r="D189" t="s">
-        <v>495</v>
+        <v>532</v>
       </c>
       <c r="E189" t="s">
         <v>487</v>
@@ -8428,7 +8436,7 @@
         <v>785</v>
       </c>
       <c r="D193" t="s">
-        <v>495</v>
+        <v>532</v>
       </c>
       <c r="E193" t="s">
         <v>487</v>
@@ -8445,7 +8453,7 @@
         <v>721</v>
       </c>
       <c r="D194" t="s">
-        <v>495</v>
+        <v>532</v>
       </c>
       <c r="E194" t="s">
         <v>502</v>
@@ -8590,7 +8598,7 @@
         <v>83</v>
       </c>
       <c r="D202" t="s">
-        <v>495</v>
+        <v>532</v>
       </c>
       <c r="E202" t="s">
         <v>487</v>
@@ -8604,19 +8612,19 @@
         <v>586</v>
       </c>
       <c r="B203" t="s">
-        <v>444</v>
+        <v>728</v>
       </c>
       <c r="C203" t="s">
-        <v>751</v>
+        <v>728</v>
       </c>
       <c r="D203" t="s">
-        <v>496</v>
-      </c>
-      <c r="E203" t="s">
-        <v>487</v>
-      </c>
-      <c r="J203" t="s">
-        <v>588</v>
+        <v>499</v>
+      </c>
+      <c r="F203" t="b">
+        <v>0</v>
+      </c>
+      <c r="G203" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:10">
@@ -8624,16 +8632,19 @@
         <v>586</v>
       </c>
       <c r="B204" t="s">
-        <v>587</v>
+        <v>444</v>
       </c>
       <c r="C204" t="s">
-        <v>587</v>
+        <v>751</v>
       </c>
       <c r="D204" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E204" t="s">
-        <v>502</v>
+        <v>487</v>
+      </c>
+      <c r="J204" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="205" spans="1:10">
@@ -8641,36 +8652,33 @@
         <v>586</v>
       </c>
       <c r="B205" t="s">
-        <v>465</v>
+        <v>587</v>
       </c>
       <c r="C205" t="s">
-        <v>466</v>
+        <v>587</v>
       </c>
       <c r="D205" t="s">
-        <v>494</v>
-      </c>
-      <c r="J205" t="s">
-        <v>589</v>
+        <v>532</v>
+      </c>
+      <c r="E205" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="206" spans="1:10">
       <c r="A206" t="s">
-        <v>703</v>
+        <v>586</v>
       </c>
       <c r="B206" t="s">
-        <v>153</v>
+        <v>465</v>
       </c>
       <c r="C206" t="s">
-        <v>703</v>
+        <v>466</v>
       </c>
       <c r="D206" t="s">
-        <v>495</v>
-      </c>
-      <c r="E206" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="J206" t="s">
-        <v>704</v>
+        <v>589</v>
       </c>
     </row>
     <row r="207" spans="1:10">
@@ -8678,99 +8686,96 @@
         <v>703</v>
       </c>
       <c r="B207" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C207" t="s">
-        <v>729</v>
+        <v>703</v>
       </c>
       <c r="D207" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="E207" t="s">
         <v>487</v>
       </c>
       <c r="J207" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="208" spans="1:10">
       <c r="A208" t="s">
         <v>703</v>
       </c>
+      <c r="B208" t="s">
+        <v>155</v>
+      </c>
       <c r="C208" t="s">
+        <v>729</v>
+      </c>
+      <c r="D208" t="s">
+        <v>496</v>
+      </c>
+      <c r="E208" t="s">
+        <v>487</v>
+      </c>
+      <c r="J208" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10">
+      <c r="A209" t="s">
+        <v>703</v>
+      </c>
+      <c r="C209" t="s">
         <v>728</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D209" t="s">
         <v>499</v>
-      </c>
-      <c r="F208" t="b">
-        <v>0</v>
-      </c>
-      <c r="G208" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="209" spans="1:10">
-      <c r="A209" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="B209" t="s">
-        <v>367</v>
-      </c>
-      <c r="C209" t="s">
-        <v>368</v>
-      </c>
-      <c r="D209" t="s">
-        <v>496</v>
-      </c>
-      <c r="E209" t="s">
-        <v>664</v>
       </c>
       <c r="F209" t="b">
         <v>0</v>
       </c>
-      <c r="J209" t="s">
-        <v>659</v>
+      <c r="G209" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:10">
       <c r="A210" s="1" t="s">
         <v>713</v>
       </c>
+      <c r="B210" t="s">
+        <v>367</v>
+      </c>
       <c r="C210" t="s">
-        <v>728</v>
+        <v>368</v>
       </c>
       <c r="D210" t="s">
-        <v>499</v>
+        <v>496</v>
+      </c>
+      <c r="E210" t="s">
+        <v>664</v>
       </c>
       <c r="F210" t="b">
         <v>0</v>
       </c>
-      <c r="G210" t="b">
-        <v>1</v>
+      <c r="J210" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="211" spans="1:10">
-      <c r="A211" t="s">
-        <v>664</v>
-      </c>
-      <c r="B211" t="s">
-        <v>369</v>
+      <c r="A211" s="1" t="s">
+        <v>713</v>
       </c>
       <c r="C211" t="s">
-        <v>370</v>
+        <v>728</v>
       </c>
       <c r="D211" t="s">
-        <v>496</v>
-      </c>
-      <c r="E211" t="s">
-        <v>661</v>
+        <v>499</v>
       </c>
       <c r="F211" t="b">
         <v>0</v>
       </c>
-      <c r="J211" t="s">
-        <v>660</v>
+      <c r="G211" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:10">
@@ -8778,10 +8783,10 @@
         <v>664</v>
       </c>
       <c r="B212" t="s">
-        <v>662</v>
+        <v>369</v>
       </c>
       <c r="C212" t="s">
-        <v>663</v>
+        <v>370</v>
       </c>
       <c r="D212" t="s">
         <v>496</v>
@@ -8793,89 +8798,95 @@
         <v>0</v>
       </c>
       <c r="J212" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
     </row>
     <row r="213" spans="1:10">
       <c r="A213" t="s">
         <v>664</v>
       </c>
+      <c r="B213" t="s">
+        <v>662</v>
+      </c>
       <c r="C213" t="s">
-        <v>728</v>
+        <v>663</v>
       </c>
       <c r="D213" t="s">
-        <v>499</v>
+        <v>496</v>
+      </c>
+      <c r="E213" t="s">
+        <v>661</v>
       </c>
       <c r="F213" t="b">
         <v>0</v>
       </c>
-      <c r="G213" t="b">
-        <v>1</v>
+      <c r="J213" t="s">
+        <v>665</v>
       </c>
     </row>
     <row r="214" spans="1:10">
       <c r="A214" t="s">
-        <v>342</v>
-      </c>
-      <c r="B214" t="s">
-        <v>343</v>
+        <v>664</v>
       </c>
       <c r="C214" t="s">
-        <v>344</v>
+        <v>728</v>
       </c>
       <c r="D214" t="s">
-        <v>532</v>
-      </c>
-      <c r="E214" t="s">
-        <v>487</v>
+        <v>499</v>
+      </c>
+      <c r="F214" t="b">
+        <v>0</v>
+      </c>
+      <c r="G214" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:10">
       <c r="A215" t="s">
         <v>342</v>
       </c>
+      <c r="B215" t="s">
+        <v>343</v>
+      </c>
       <c r="C215" t="s">
-        <v>728</v>
+        <v>344</v>
       </c>
       <c r="D215" t="s">
-        <v>499</v>
-      </c>
-      <c r="F215" t="b">
-        <v>0</v>
-      </c>
-      <c r="G215" t="b">
-        <v>1</v>
+        <v>532</v>
+      </c>
+      <c r="E215" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="216" spans="1:10">
       <c r="A216" t="s">
         <v>342</v>
       </c>
-      <c r="B216" t="s">
-        <v>342</v>
-      </c>
       <c r="C216" t="s">
-        <v>342</v>
+        <v>728</v>
       </c>
       <c r="D216" t="s">
-        <v>497</v>
+        <v>499</v>
+      </c>
+      <c r="F216" t="b">
+        <v>0</v>
+      </c>
+      <c r="G216" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:10">
       <c r="A217" t="s">
-        <v>716</v>
+        <v>342</v>
       </c>
       <c r="B217" t="s">
-        <v>154</v>
+        <v>342</v>
       </c>
       <c r="C217" t="s">
-        <v>782</v>
+        <v>342</v>
       </c>
       <c r="D217" t="s">
-        <v>532</v>
-      </c>
-      <c r="E217" t="s">
-        <v>487</v>
+        <v>497</v>
       </c>
     </row>
     <row r="218" spans="1:10">
@@ -8883,13 +8894,16 @@
         <v>716</v>
       </c>
       <c r="B218" t="s">
-        <v>243</v>
+        <v>154</v>
       </c>
       <c r="C218" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D218" t="s">
-        <v>497</v>
+        <v>532</v>
+      </c>
+      <c r="E218" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="219" spans="1:10">
@@ -8897,10 +8911,10 @@
         <v>716</v>
       </c>
       <c r="B219" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C219" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D219" t="s">
         <v>497</v>
@@ -8911,10 +8925,10 @@
         <v>716</v>
       </c>
       <c r="B220" t="s">
-        <v>355</v>
+        <v>237</v>
       </c>
       <c r="C220" t="s">
-        <v>356</v>
+        <v>784</v>
       </c>
       <c r="D220" t="s">
         <v>497</v>
@@ -8925,13 +8939,13 @@
         <v>716</v>
       </c>
       <c r="B221" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C221" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D221" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="222" spans="1:10">
@@ -8939,13 +8953,13 @@
         <v>716</v>
       </c>
       <c r="B222" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="C222" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="D222" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="223" spans="1:10">
@@ -8953,10 +8967,10 @@
         <v>716</v>
       </c>
       <c r="B223" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C223" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D223" t="s">
         <v>499</v>
@@ -8967,13 +8981,13 @@
         <v>716</v>
       </c>
       <c r="B224" t="s">
-        <v>426</v>
+        <v>349</v>
       </c>
       <c r="C224" t="s">
-        <v>427</v>
+        <v>350</v>
       </c>
       <c r="D224" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="225" spans="1:10">
@@ -8981,16 +8995,13 @@
         <v>716</v>
       </c>
       <c r="B225" t="s">
-        <v>357</v>
+        <v>426</v>
       </c>
       <c r="C225" t="s">
-        <v>358</v>
+        <v>427</v>
       </c>
       <c r="D225" t="s">
-        <v>496</v>
-      </c>
-      <c r="E225" t="s">
-        <v>240</v>
+        <v>497</v>
       </c>
     </row>
     <row r="226" spans="1:10">
@@ -8998,13 +9009,16 @@
         <v>716</v>
       </c>
       <c r="B226" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="C226" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="D226" t="s">
-        <v>499</v>
+        <v>496</v>
+      </c>
+      <c r="E226" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="227" spans="1:10">
@@ -9012,10 +9026,10 @@
         <v>716</v>
       </c>
       <c r="B227" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C227" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D227" t="s">
         <v>499</v>
@@ -9025,31 +9039,25 @@
       <c r="A228" t="s">
         <v>716</v>
       </c>
+      <c r="B228" t="s">
+        <v>353</v>
+      </c>
       <c r="C228" t="s">
-        <v>728</v>
+        <v>354</v>
       </c>
       <c r="D228" t="s">
         <v>499</v>
       </c>
-      <c r="F228" t="b">
-        <v>0</v>
-      </c>
-      <c r="G228" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="229" spans="1:10">
       <c r="A229" t="s">
-        <v>714</v>
-      </c>
-      <c r="B229" t="s">
-        <v>372</v>
+        <v>716</v>
       </c>
       <c r="C229" t="s">
-        <v>373</v>
+        <v>728</v>
       </c>
       <c r="D229" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="F229" t="b">
         <v>0</v>
@@ -9063,16 +9071,19 @@
         <v>714</v>
       </c>
       <c r="B230" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="C230" t="s">
-        <v>692</v>
+        <v>373</v>
       </c>
       <c r="D230" t="s">
-        <v>496</v>
-      </c>
-      <c r="E230" t="s">
-        <v>675</v>
+        <v>491</v>
+      </c>
+      <c r="F230" t="b">
+        <v>0</v>
+      </c>
+      <c r="G230" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:10">
@@ -9080,36 +9091,33 @@
         <v>714</v>
       </c>
       <c r="B231" t="s">
-        <v>715</v>
+        <v>386</v>
       </c>
       <c r="C231" t="s">
-        <v>502</v>
+        <v>692</v>
       </c>
       <c r="D231" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E231" t="s">
-        <v>502</v>
+        <v>675</v>
       </c>
     </row>
     <row r="232" spans="1:10">
       <c r="A232" t="s">
-        <v>533</v>
+        <v>714</v>
       </c>
       <c r="B232" t="s">
-        <v>458</v>
+        <v>715</v>
       </c>
       <c r="C232" t="s">
-        <v>545</v>
+        <v>502</v>
       </c>
       <c r="D232" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="E232" t="s">
-        <v>545</v>
-      </c>
-      <c r="J232" t="s">
-        <v>544</v>
+        <v>502</v>
       </c>
     </row>
     <row r="233" spans="1:10">
@@ -9117,22 +9125,19 @@
         <v>533</v>
       </c>
       <c r="B233" t="s">
-        <v>151</v>
+        <v>458</v>
       </c>
       <c r="C233" t="s">
-        <v>502</v>
+        <v>545</v>
       </c>
       <c r="D233" t="s">
         <v>496</v>
       </c>
       <c r="E233" t="s">
-        <v>502</v>
-      </c>
-      <c r="F233" t="b">
-        <v>0</v>
+        <v>545</v>
       </c>
       <c r="J233" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
     </row>
     <row r="234" spans="1:10">
@@ -9140,16 +9145,22 @@
         <v>533</v>
       </c>
       <c r="B234" t="s">
-        <v>252</v>
+        <v>151</v>
       </c>
       <c r="C234" t="s">
-        <v>253</v>
+        <v>502</v>
       </c>
       <c r="D234" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="E234" t="s">
+        <v>502</v>
+      </c>
+      <c r="F234" t="b">
+        <v>0</v>
       </c>
       <c r="J234" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="235" spans="1:10">
@@ -9157,19 +9168,16 @@
         <v>533</v>
       </c>
       <c r="B235" t="s">
-        <v>457</v>
+        <v>252</v>
       </c>
       <c r="C235" t="s">
-        <v>541</v>
+        <v>253</v>
       </c>
       <c r="D235" t="s">
-        <v>496</v>
-      </c>
-      <c r="E235" t="s">
-        <v>541</v>
+        <v>491</v>
       </c>
       <c r="J235" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="236" spans="1:10">
@@ -9177,56 +9185,59 @@
         <v>533</v>
       </c>
       <c r="B236" t="s">
-        <v>250</v>
+        <v>457</v>
       </c>
       <c r="C236" t="s">
-        <v>251</v>
+        <v>541</v>
       </c>
       <c r="D236" t="s">
-        <v>491</v>
-      </c>
-      <c r="F236" t="b">
-        <v>0</v>
-      </c>
-      <c r="G236" t="b">
-        <v>1</v>
+        <v>496</v>
+      </c>
+      <c r="E236" t="s">
+        <v>541</v>
       </c>
       <c r="J236" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
     </row>
     <row r="237" spans="1:10">
       <c r="A237" t="s">
         <v>533</v>
       </c>
-      <c r="B237" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C237" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="D237" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="H237" t="s">
-        <v>534</v>
+      <c r="B237" t="s">
+        <v>250</v>
+      </c>
+      <c r="C237" t="s">
+        <v>251</v>
+      </c>
+      <c r="D237" t="s">
+        <v>491</v>
+      </c>
+      <c r="F237" t="b">
+        <v>0</v>
+      </c>
+      <c r="G237" t="b">
+        <v>1</v>
+      </c>
+      <c r="J237" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="238" spans="1:10">
       <c r="A238" t="s">
         <v>533</v>
       </c>
-      <c r="B238" t="s">
-        <v>459</v>
-      </c>
-      <c r="C238" t="s">
-        <v>548</v>
-      </c>
-      <c r="D238" t="s">
-        <v>496</v>
-      </c>
-      <c r="E238" t="s">
-        <v>548</v>
+      <c r="B238" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="H238" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="239" spans="1:10">
@@ -9234,39 +9245,36 @@
         <v>533</v>
       </c>
       <c r="B239" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C239" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D239" t="s">
         <v>496</v>
       </c>
       <c r="E239" t="s">
-        <v>551</v>
-      </c>
-      <c r="J239" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="240" spans="1:10">
       <c r="A240" t="s">
-        <v>502</v>
+        <v>533</v>
       </c>
       <c r="B240" t="s">
-        <v>147</v>
+        <v>460</v>
       </c>
       <c r="C240" t="s">
-        <v>148</v>
+        <v>551</v>
       </c>
       <c r="D240" t="s">
-        <v>491</v>
-      </c>
-      <c r="F240" t="b">
-        <v>0</v>
-      </c>
-      <c r="G240" t="b">
-        <v>1</v>
+        <v>496</v>
+      </c>
+      <c r="E240" t="s">
+        <v>551</v>
+      </c>
+      <c r="J240" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="241" spans="1:10">
@@ -9274,13 +9282,19 @@
         <v>502</v>
       </c>
       <c r="B241" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C241" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D241" t="s">
         <v>491</v>
+      </c>
+      <c r="F241" t="b">
+        <v>0</v>
+      </c>
+      <c r="G241" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="242" spans="1:10">
@@ -9288,16 +9302,13 @@
         <v>502</v>
       </c>
       <c r="B242" t="s">
-        <v>449</v>
+        <v>145</v>
       </c>
       <c r="C242" t="s">
-        <v>450</v>
+        <v>146</v>
       </c>
       <c r="D242" t="s">
-        <v>494</v>
-      </c>
-      <c r="J242" t="s">
-        <v>540</v>
+        <v>491</v>
       </c>
     </row>
     <row r="243" spans="1:10">
@@ -9305,16 +9316,16 @@
         <v>502</v>
       </c>
       <c r="B243" t="s">
-        <v>149</v>
+        <v>449</v>
       </c>
       <c r="C243" t="s">
-        <v>150</v>
+        <v>450</v>
       </c>
       <c r="D243" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="J243" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="244" spans="1:10">
@@ -9322,30 +9333,33 @@
         <v>502</v>
       </c>
       <c r="B244" t="s">
-        <v>474</v>
+        <v>149</v>
       </c>
       <c r="C244" t="s">
-        <v>475</v>
+        <v>150</v>
       </c>
       <c r="D244" t="s">
         <v>499</v>
       </c>
       <c r="J244" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="245" spans="1:10">
       <c r="A245" t="s">
-        <v>725</v>
+        <v>502</v>
       </c>
       <c r="B245" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C245" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D245" t="s">
-        <v>491</v>
+        <v>499</v>
+      </c>
+      <c r="J245" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="246" spans="1:10">
@@ -9353,13 +9367,19 @@
         <v>725</v>
       </c>
       <c r="B246" t="s">
-        <v>74</v>
+        <v>728</v>
       </c>
       <c r="C246" t="s">
-        <v>75</v>
+        <v>728</v>
       </c>
       <c r="D246" t="s">
-        <v>491</v>
+        <v>499</v>
+      </c>
+      <c r="F246" t="b">
+        <v>0</v>
+      </c>
+      <c r="G246" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="247" spans="1:10">
@@ -9367,10 +9387,10 @@
         <v>725</v>
       </c>
       <c r="B247" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="C247" t="s">
-        <v>454</v>
+        <v>477</v>
       </c>
       <c r="D247" t="s">
         <v>491</v>
@@ -9381,10 +9401,10 @@
         <v>725</v>
       </c>
       <c r="B248" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C248" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D248" t="s">
         <v>491</v>
@@ -9395,16 +9415,13 @@
         <v>725</v>
       </c>
       <c r="B249" t="s">
-        <v>715</v>
+        <v>453</v>
       </c>
       <c r="C249" t="s">
-        <v>502</v>
+        <v>454</v>
       </c>
       <c r="D249" t="s">
-        <v>495</v>
-      </c>
-      <c r="E249" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
     </row>
     <row r="250" spans="1:10">
@@ -9412,13 +9429,13 @@
         <v>725</v>
       </c>
       <c r="B250" t="s">
-        <v>451</v>
+        <v>72</v>
       </c>
       <c r="C250" t="s">
-        <v>452</v>
+        <v>73</v>
       </c>
       <c r="D250" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
     </row>
     <row r="251" spans="1:10">
@@ -9426,44 +9443,41 @@
         <v>725</v>
       </c>
       <c r="B251" t="s">
-        <v>478</v>
+        <v>715</v>
       </c>
       <c r="C251" t="s">
-        <v>479</v>
+        <v>502</v>
       </c>
       <c r="D251" t="s">
-        <v>491</v>
+        <v>532</v>
+      </c>
+      <c r="E251" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="252" spans="1:10">
       <c r="A252" t="s">
-        <v>706</v>
+        <v>725</v>
       </c>
       <c r="B252" t="s">
-        <v>404</v>
+        <v>451</v>
       </c>
       <c r="C252" t="s">
-        <v>781</v>
+        <v>452</v>
       </c>
       <c r="D252" t="s">
-        <v>496</v>
-      </c>
-      <c r="E252" t="s">
-        <v>487</v>
-      </c>
-      <c r="F252" t="b">
-        <v>0</v>
+        <v>501</v>
       </c>
     </row>
     <row r="253" spans="1:10">
       <c r="A253" t="s">
-        <v>706</v>
+        <v>725</v>
       </c>
       <c r="B253" t="s">
-        <v>396</v>
+        <v>478</v>
       </c>
       <c r="C253" t="s">
-        <v>780</v>
+        <v>479</v>
       </c>
       <c r="D253" t="s">
         <v>491</v>
@@ -9474,16 +9488,19 @@
         <v>706</v>
       </c>
       <c r="B254" t="s">
-        <v>264</v>
+        <v>404</v>
       </c>
       <c r="C254" t="s">
-        <v>487</v>
+        <v>781</v>
       </c>
       <c r="D254" t="s">
         <v>496</v>
       </c>
       <c r="E254" t="s">
         <v>487</v>
+      </c>
+      <c r="F254" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:10">
@@ -9491,10 +9508,10 @@
         <v>706</v>
       </c>
       <c r="B255" t="s">
-        <v>262</v>
+        <v>396</v>
       </c>
       <c r="C255" t="s">
-        <v>753</v>
+        <v>780</v>
       </c>
       <c r="D255" t="s">
         <v>491</v>
@@ -9505,13 +9522,16 @@
         <v>706</v>
       </c>
       <c r="B256" t="s">
-        <v>398</v>
+        <v>264</v>
       </c>
       <c r="C256" t="s">
-        <v>779</v>
+        <v>487</v>
       </c>
       <c r="D256" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="E256" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="257" spans="1:10">
@@ -9519,13 +9539,13 @@
         <v>706</v>
       </c>
       <c r="B257" t="s">
-        <v>413</v>
+        <v>262</v>
       </c>
       <c r="C257" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="D257" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="258" spans="1:10">
@@ -9533,16 +9553,13 @@
         <v>706</v>
       </c>
       <c r="B258" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C258" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="D258" t="s">
-        <v>524</v>
-      </c>
-      <c r="H258" t="s">
-        <v>707</v>
+        <v>491</v>
       </c>
     </row>
     <row r="259" spans="1:10">
@@ -9550,13 +9567,13 @@
         <v>706</v>
       </c>
       <c r="B259" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="C259" t="s">
-        <v>778</v>
+        <v>747</v>
       </c>
       <c r="D259" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="260" spans="1:10">
@@ -9564,13 +9581,16 @@
         <v>706</v>
       </c>
       <c r="B260" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C260" t="s">
-        <v>743</v>
+        <v>777</v>
       </c>
       <c r="D260" t="s">
-        <v>491</v>
+        <v>524</v>
+      </c>
+      <c r="H260" t="s">
+        <v>707</v>
       </c>
     </row>
     <row r="261" spans="1:10">
@@ -9578,16 +9598,13 @@
         <v>706</v>
       </c>
       <c r="B261" t="s">
-        <v>136</v>
+        <v>399</v>
       </c>
       <c r="C261" t="s">
-        <v>137</v>
+        <v>778</v>
       </c>
       <c r="D261" t="s">
-        <v>496</v>
-      </c>
-      <c r="E261" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
     </row>
     <row r="262" spans="1:10">
@@ -9595,16 +9612,13 @@
         <v>706</v>
       </c>
       <c r="B262" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C262" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="D262" t="s">
-        <v>496</v>
-      </c>
-      <c r="E262" t="s">
-        <v>616</v>
+        <v>491</v>
       </c>
     </row>
     <row r="263" spans="1:10">
@@ -9612,19 +9626,16 @@
         <v>706</v>
       </c>
       <c r="B263" t="s">
-        <v>394</v>
+        <v>136</v>
       </c>
       <c r="C263" t="s">
-        <v>395</v>
+        <v>137</v>
       </c>
       <c r="D263" t="s">
-        <v>491</v>
-      </c>
-      <c r="F263" t="b">
-        <v>0</v>
-      </c>
-      <c r="G263" t="b">
-        <v>1</v>
+        <v>496</v>
+      </c>
+      <c r="E263" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="264" spans="1:10">
@@ -9632,13 +9643,16 @@
         <v>706</v>
       </c>
       <c r="B264" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="C264" t="s">
-        <v>401</v>
+        <v>742</v>
       </c>
       <c r="D264" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="E264" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="265" spans="1:10">
@@ -9646,13 +9660,19 @@
         <v>706</v>
       </c>
       <c r="B265" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="C265" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="D265" t="s">
         <v>491</v>
+      </c>
+      <c r="F265" t="b">
+        <v>0</v>
+      </c>
+      <c r="G265" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="266" spans="1:10">
@@ -9660,10 +9680,10 @@
         <v>706</v>
       </c>
       <c r="B266" t="s">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="C266" t="s">
-        <v>251</v>
+        <v>401</v>
       </c>
       <c r="D266" t="s">
         <v>491</v>
@@ -9674,13 +9694,13 @@
         <v>706</v>
       </c>
       <c r="B267" t="s">
-        <v>65</v>
+        <v>402</v>
       </c>
       <c r="C267" t="s">
-        <v>66</v>
+        <v>403</v>
       </c>
       <c r="D267" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="268" spans="1:10">
@@ -9688,50 +9708,41 @@
         <v>706</v>
       </c>
       <c r="B268" t="s">
-        <v>67</v>
+        <v>250</v>
       </c>
       <c r="C268" t="s">
-        <v>68</v>
+        <v>251</v>
       </c>
       <c r="D268" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="269" spans="1:10">
       <c r="A269" t="s">
-        <v>629</v>
+        <v>706</v>
       </c>
       <c r="B269" t="s">
-        <v>304</v>
+        <v>65</v>
       </c>
       <c r="C269" t="s">
-        <v>750</v>
+        <v>66</v>
       </c>
       <c r="D269" t="s">
-        <v>496</v>
-      </c>
-      <c r="E269" t="s">
-        <v>616</v>
-      </c>
-      <c r="J269" t="s">
-        <v>637</v>
+        <v>498</v>
       </c>
     </row>
     <row r="270" spans="1:10">
       <c r="A270" t="s">
-        <v>629</v>
+        <v>706</v>
       </c>
       <c r="B270" t="s">
-        <v>366</v>
+        <v>67</v>
       </c>
       <c r="C270" t="s">
-        <v>747</v>
+        <v>68</v>
       </c>
       <c r="D270" t="s">
-        <v>494</v>
-      </c>
-      <c r="J270" t="s">
-        <v>669</v>
+        <v>492</v>
       </c>
     </row>
     <row r="271" spans="1:10">
@@ -9739,16 +9750,19 @@
         <v>629</v>
       </c>
       <c r="B271" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C271" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="D271" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="E271" t="s">
+        <v>616</v>
       </c>
       <c r="J271" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="272" spans="1:10">
@@ -9756,13 +9770,16 @@
         <v>629</v>
       </c>
       <c r="B272" t="s">
-        <v>299</v>
+        <v>366</v>
       </c>
       <c r="C272" t="s">
-        <v>124</v>
+        <v>747</v>
       </c>
       <c r="D272" t="s">
-        <v>491</v>
+        <v>494</v>
+      </c>
+      <c r="J272" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="273" spans="1:10">
@@ -9770,16 +9787,16 @@
         <v>629</v>
       </c>
       <c r="B273" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C273" t="s">
-        <v>787</v>
+        <v>753</v>
       </c>
       <c r="D273" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="J273" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
     </row>
     <row r="274" spans="1:10">
@@ -9787,16 +9804,13 @@
         <v>629</v>
       </c>
       <c r="B274" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C274" t="s">
-        <v>788</v>
+        <v>124</v>
       </c>
       <c r="D274" t="s">
-        <v>492</v>
-      </c>
-      <c r="J274" t="s">
-        <v>634</v>
+        <v>491</v>
       </c>
     </row>
     <row r="275" spans="1:10">
@@ -9804,16 +9818,16 @@
         <v>629</v>
       </c>
       <c r="B275" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="C275" t="s">
-        <v>778</v>
+        <v>787</v>
       </c>
       <c r="D275" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="J275" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="276" spans="1:10">
@@ -9821,16 +9835,16 @@
         <v>629</v>
       </c>
       <c r="B276" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C276" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D276" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="J276" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="277" spans="1:10">
@@ -9838,16 +9852,16 @@
         <v>629</v>
       </c>
       <c r="B277" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C277" t="s">
-        <v>791</v>
+        <v>778</v>
       </c>
       <c r="D277" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J277" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="278" spans="1:10">
@@ -9855,42 +9869,33 @@
         <v>629</v>
       </c>
       <c r="B278" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="C278" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D278" t="s">
-        <v>524</v>
-      </c>
-      <c r="H278" t="s">
-        <v>667</v>
+        <v>498</v>
       </c>
       <c r="J278" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="279" spans="1:10" ht="16" customHeight="1">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10">
       <c r="A279" t="s">
         <v>629</v>
       </c>
       <c r="B279" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C279" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="D279" t="s">
-        <v>496</v>
-      </c>
-      <c r="E279" t="s">
-        <v>640</v>
-      </c>
-      <c r="F279" t="b">
-        <v>0</v>
+        <v>492</v>
       </c>
       <c r="J279" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="280" spans="1:10">
@@ -9898,39 +9903,42 @@
         <v>629</v>
       </c>
       <c r="B280" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="C280" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D280" t="s">
-        <v>491</v>
-      </c>
-      <c r="F280" t="b">
-        <v>0</v>
-      </c>
-      <c r="G280" t="b">
-        <v>1</v>
+        <v>524</v>
+      </c>
+      <c r="H280" t="s">
+        <v>667</v>
       </c>
       <c r="J280" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="281" spans="1:10">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" ht="16" customHeight="1">
       <c r="A281" t="s">
         <v>629</v>
       </c>
       <c r="B281" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="C281" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="D281" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="E281" t="s">
+        <v>640</v>
+      </c>
+      <c r="F281" t="b">
+        <v>0</v>
       </c>
       <c r="J281" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
     </row>
     <row r="282" spans="1:10">
@@ -9938,16 +9946,22 @@
         <v>629</v>
       </c>
       <c r="B282" t="s">
-        <v>265</v>
+        <v>302</v>
       </c>
       <c r="C282" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="D282" t="s">
         <v>491</v>
       </c>
+      <c r="F282" t="b">
+        <v>0</v>
+      </c>
+      <c r="G282" t="b">
+        <v>1</v>
+      </c>
       <c r="J282" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="283" spans="1:10">
@@ -9955,16 +9969,16 @@
         <v>629</v>
       </c>
       <c r="B283" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="C283" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="D283" t="s">
         <v>491</v>
       </c>
       <c r="J283" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="284" spans="1:10">
@@ -9972,16 +9986,16 @@
         <v>629</v>
       </c>
       <c r="B284" t="s">
-        <v>307</v>
+        <v>265</v>
       </c>
       <c r="C284" t="s">
-        <v>308</v>
+        <v>798</v>
       </c>
       <c r="D284" t="s">
         <v>491</v>
       </c>
       <c r="J284" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="285" spans="1:10">
@@ -9989,16 +10003,16 @@
         <v>629</v>
       </c>
       <c r="B285" t="s">
-        <v>76</v>
+        <v>305</v>
       </c>
       <c r="C285" t="s">
-        <v>76</v>
+        <v>799</v>
       </c>
       <c r="D285" t="s">
         <v>491</v>
       </c>
       <c r="J285" t="s">
-        <v>670</v>
+        <v>631</v>
       </c>
     </row>
     <row r="286" spans="1:10">
@@ -10006,69 +10020,63 @@
         <v>629</v>
       </c>
       <c r="B286" t="s">
-        <v>208</v>
+        <v>307</v>
       </c>
       <c r="C286" t="s">
-        <v>209</v>
+        <v>308</v>
       </c>
       <c r="D286" t="s">
-        <v>524</v>
-      </c>
-      <c r="H286" t="s">
-        <v>673</v>
+        <v>491</v>
+      </c>
+      <c r="J286" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="287" spans="1:10">
       <c r="A287" t="s">
-        <v>640</v>
+        <v>629</v>
+      </c>
+      <c r="B287" t="s">
+        <v>76</v>
       </c>
       <c r="C287" t="s">
-        <v>728</v>
+        <v>76</v>
       </c>
       <c r="D287" t="s">
-        <v>499</v>
-      </c>
-      <c r="E287" s="1"/>
-      <c r="F287" t="b">
-        <v>0</v>
-      </c>
-      <c r="G287" t="b">
-        <v>1</v>
+        <v>491</v>
+      </c>
+      <c r="J287" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="288" spans="1:10">
       <c r="A288" t="s">
+        <v>629</v>
+      </c>
+      <c r="B288" t="s">
+        <v>208</v>
+      </c>
+      <c r="C288" t="s">
+        <v>209</v>
+      </c>
+      <c r="D288" t="s">
+        <v>524</v>
+      </c>
+      <c r="H288" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10">
+      <c r="A289" t="s">
         <v>640</v>
       </c>
-      <c r="B288" t="s">
-        <v>301</v>
-      </c>
-      <c r="C288" t="s">
-        <v>640</v>
-      </c>
-      <c r="D288" t="s">
-        <v>496</v>
-      </c>
-      <c r="E288" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="J288" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="289" spans="1:7">
-      <c r="A289" t="s">
-        <v>710</v>
-      </c>
-      <c r="B289" t="s">
-        <v>421</v>
-      </c>
       <c r="C289" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="D289" t="s">
-        <v>491</v>
-      </c>
+        <v>499</v>
+      </c>
+      <c r="E289" s="1"/>
       <c r="F289" t="b">
         <v>0</v>
       </c>
@@ -10076,94 +10084,100 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:7">
+    <row r="290" spans="1:10">
       <c r="A290" t="s">
-        <v>710</v>
+        <v>640</v>
       </c>
       <c r="B290" t="s">
-        <v>422</v>
+        <v>301</v>
       </c>
       <c r="C290" t="s">
-        <v>738</v>
+        <v>640</v>
       </c>
       <c r="D290" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="291" spans="1:7">
+        <v>496</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="J290" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10">
       <c r="A291" t="s">
         <v>710</v>
       </c>
       <c r="B291" t="s">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="C291" t="s">
-        <v>753</v>
+        <v>736</v>
       </c>
       <c r="D291" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="292" spans="1:7">
+      <c r="F291" t="b">
+        <v>0</v>
+      </c>
+      <c r="G291" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10">
       <c r="A292" t="s">
         <v>710</v>
       </c>
       <c r="B292" t="s">
-        <v>301</v>
+        <v>422</v>
       </c>
       <c r="C292" t="s">
-        <v>764</v>
+        <v>738</v>
       </c>
       <c r="D292" t="s">
-        <v>496</v>
-      </c>
-      <c r="E292" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="293" spans="1:7">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10">
       <c r="A293" t="s">
         <v>710</v>
       </c>
       <c r="B293" t="s">
-        <v>71</v>
+        <v>300</v>
       </c>
       <c r="C293" t="s">
-        <v>733</v>
+        <v>753</v>
       </c>
       <c r="D293" t="s">
-        <v>495</v>
-      </c>
-      <c r="E293" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="294" spans="1:7">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10">
       <c r="A294" t="s">
         <v>710</v>
       </c>
       <c r="B294" t="s">
-        <v>264</v>
+        <v>301</v>
       </c>
       <c r="C294" t="s">
-        <v>706</v>
+        <v>764</v>
       </c>
       <c r="D294" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E294" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="295" spans="1:7">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10">
       <c r="A295" t="s">
         <v>710</v>
       </c>
       <c r="B295" t="s">
-        <v>310</v>
+        <v>71</v>
       </c>
       <c r="C295" t="s">
-        <v>765</v>
+        <v>733</v>
       </c>
       <c r="D295" t="s">
         <v>532</v>
@@ -10172,142 +10186,142 @@
         <v>489</v>
       </c>
     </row>
-    <row r="296" spans="1:7">
+    <row r="296" spans="1:10">
       <c r="A296" t="s">
         <v>710</v>
       </c>
       <c r="B296" t="s">
-        <v>311</v>
+        <v>264</v>
       </c>
       <c r="C296" t="s">
-        <v>766</v>
+        <v>706</v>
       </c>
       <c r="D296" t="s">
         <v>532</v>
       </c>
       <c r="E296" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="297" spans="1:7">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10">
       <c r="A297" t="s">
         <v>710</v>
       </c>
       <c r="B297" t="s">
-        <v>262</v>
+        <v>310</v>
       </c>
       <c r="C297" t="s">
-        <v>263</v>
+        <v>765</v>
       </c>
       <c r="D297" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="298" spans="1:7">
+        <v>532</v>
+      </c>
+      <c r="E297" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10">
       <c r="A298" t="s">
         <v>710</v>
       </c>
       <c r="B298" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="C298" t="s">
-        <v>303</v>
+        <v>766</v>
       </c>
       <c r="D298" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="299" spans="1:7">
+        <v>532</v>
+      </c>
+      <c r="E298" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10">
       <c r="A299" t="s">
         <v>710</v>
       </c>
       <c r="B299" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
       <c r="C299" t="s">
-        <v>137</v>
+        <v>263</v>
       </c>
       <c r="D299" t="s">
-        <v>495</v>
-      </c>
-      <c r="E299" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="300" spans="1:7">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10">
       <c r="A300" t="s">
         <v>710</v>
       </c>
       <c r="B300" t="s">
-        <v>394</v>
+        <v>302</v>
       </c>
       <c r="C300" t="s">
-        <v>395</v>
+        <v>303</v>
       </c>
       <c r="D300" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="301" spans="1:7">
+    <row r="301" spans="1:10">
       <c r="A301" t="s">
         <v>710</v>
       </c>
       <c r="B301" t="s">
-        <v>250</v>
+        <v>136</v>
       </c>
       <c r="C301" t="s">
-        <v>251</v>
+        <v>137</v>
       </c>
       <c r="D301" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="302" spans="1:7">
+        <v>532</v>
+      </c>
+      <c r="E301" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10">
       <c r="A302" t="s">
         <v>710</v>
       </c>
       <c r="B302" t="s">
+        <v>394</v>
+      </c>
+      <c r="C302" t="s">
+        <v>395</v>
+      </c>
+      <c r="D302" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10">
+      <c r="A303" t="s">
+        <v>710</v>
+      </c>
+      <c r="B303" t="s">
+        <v>250</v>
+      </c>
+      <c r="C303" t="s">
+        <v>251</v>
+      </c>
+      <c r="D303" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10">
+      <c r="A304" t="s">
+        <v>710</v>
+      </c>
+      <c r="B304" t="s">
         <v>69</v>
       </c>
-      <c r="C302" t="s">
+      <c r="C304" t="s">
         <v>70</v>
       </c>
-      <c r="D302" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="303" spans="1:7">
-      <c r="A303" t="s">
-        <v>14</v>
-      </c>
-      <c r="B303" t="s">
-        <v>321</v>
-      </c>
-      <c r="C303" t="s">
-        <v>744</v>
-      </c>
-      <c r="D303" t="s">
-        <v>496</v>
-      </c>
-      <c r="E303" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="304" spans="1:7">
-      <c r="A304" t="s">
-        <v>14</v>
-      </c>
-      <c r="B304" t="s">
-        <v>125</v>
-      </c>
-      <c r="C304" t="s">
-        <v>750</v>
-      </c>
       <c r="D304" t="s">
-        <v>496</v>
-      </c>
-      <c r="E304" t="s">
-        <v>616</v>
+        <v>491</v>
       </c>
     </row>
     <row r="305" spans="1:10">
@@ -10315,16 +10329,16 @@
         <v>14</v>
       </c>
       <c r="B305" t="s">
-        <v>143</v>
+        <v>321</v>
       </c>
       <c r="C305" t="s">
-        <v>144</v>
+        <v>744</v>
       </c>
       <c r="D305" t="s">
         <v>496</v>
       </c>
       <c r="E305" t="s">
-        <v>714</v>
+        <v>502</v>
       </c>
     </row>
     <row r="306" spans="1:10">
@@ -10332,10 +10346,10 @@
         <v>14</v>
       </c>
       <c r="B306" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C306" t="s">
-        <v>131</v>
+        <v>750</v>
       </c>
       <c r="D306" t="s">
         <v>496</v>
@@ -10349,16 +10363,16 @@
         <v>14</v>
       </c>
       <c r="B307" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="C307" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="D307" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E307" t="s">
-        <v>487</v>
+        <v>714</v>
       </c>
     </row>
     <row r="308" spans="1:10">
@@ -10366,13 +10380,16 @@
         <v>14</v>
       </c>
       <c r="B308" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C308" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D308" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="E308" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="309" spans="1:10">
@@ -10380,19 +10397,16 @@
         <v>14</v>
       </c>
       <c r="B309" t="s">
-        <v>252</v>
+        <v>118</v>
       </c>
       <c r="C309" t="s">
-        <v>253</v>
+        <v>119</v>
       </c>
       <c r="D309" t="s">
-        <v>491</v>
-      </c>
-      <c r="F309" t="b">
-        <v>0</v>
-      </c>
-      <c r="G309" t="b">
-        <v>1</v>
+        <v>532</v>
+      </c>
+      <c r="E309" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="310" spans="1:10">
@@ -10400,10 +10414,10 @@
         <v>14</v>
       </c>
       <c r="B310" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C310" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D310" t="s">
         <v>491</v>
@@ -10414,13 +10428,19 @@
         <v>14</v>
       </c>
       <c r="B311" t="s">
-        <v>447</v>
+        <v>252</v>
       </c>
       <c r="C311" t="s">
-        <v>448</v>
+        <v>253</v>
       </c>
       <c r="D311" t="s">
-        <v>493</v>
+        <v>491</v>
+      </c>
+      <c r="F311" t="b">
+        <v>0</v>
+      </c>
+      <c r="G311" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="312" spans="1:10">
@@ -10428,10 +10448,10 @@
         <v>14</v>
       </c>
       <c r="B312" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="C312" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="D312" t="s">
         <v>491</v>
@@ -10442,13 +10462,13 @@
         <v>14</v>
       </c>
       <c r="B313" t="s">
-        <v>128</v>
+        <v>447</v>
       </c>
       <c r="C313" t="s">
-        <v>129</v>
+        <v>448</v>
       </c>
       <c r="D313" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="314" spans="1:10">
@@ -10456,10 +10476,10 @@
         <v>14</v>
       </c>
       <c r="B314" t="s">
-        <v>236</v>
+        <v>72</v>
       </c>
       <c r="C314" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="D314" t="s">
         <v>491</v>
@@ -10467,82 +10487,67 @@
     </row>
     <row r="315" spans="1:10">
       <c r="A315" t="s">
-        <v>724</v>
+        <v>14</v>
       </c>
       <c r="B315" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="C315" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="D315" t="s">
-        <v>496</v>
-      </c>
-      <c r="E315" t="s">
-        <v>725</v>
+        <v>491</v>
       </c>
     </row>
     <row r="316" spans="1:10">
       <c r="A316" t="s">
-        <v>724</v>
+        <v>14</v>
       </c>
       <c r="B316" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="C316" t="s">
-        <v>253</v>
+        <v>56</v>
       </c>
       <c r="D316" t="s">
         <v>491</v>
-      </c>
-      <c r="F316" t="b">
-        <v>0</v>
-      </c>
-      <c r="G316" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:10">
       <c r="A317" t="s">
-        <v>675</v>
+        <v>724</v>
       </c>
       <c r="B317" t="s">
-        <v>386</v>
+        <v>151</v>
       </c>
       <c r="C317" t="s">
-        <v>387</v>
+        <v>152</v>
       </c>
       <c r="D317" t="s">
         <v>496</v>
       </c>
       <c r="E317" t="s">
-        <v>692</v>
-      </c>
-      <c r="F317" t="b">
-        <v>0</v>
-      </c>
-      <c r="J317" t="s">
-        <v>693</v>
+        <v>725</v>
       </c>
     </row>
     <row r="318" spans="1:10">
       <c r="A318" t="s">
-        <v>675</v>
+        <v>724</v>
       </c>
       <c r="B318" t="s">
-        <v>375</v>
+        <v>252</v>
       </c>
       <c r="C318" t="s">
-        <v>376</v>
+        <v>253</v>
       </c>
       <c r="D318" t="s">
-        <v>496</v>
-      </c>
-      <c r="E318" t="s">
-        <v>373</v>
-      </c>
-      <c r="J318" t="s">
-        <v>678</v>
+        <v>491</v>
+      </c>
+      <c r="F318" t="b">
+        <v>0</v>
+      </c>
+      <c r="G318" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:10">
@@ -10550,22 +10555,19 @@
         <v>675</v>
       </c>
       <c r="B319" t="s">
-        <v>381</v>
+        <v>728</v>
       </c>
       <c r="C319" t="s">
-        <v>382</v>
+        <v>728</v>
       </c>
       <c r="D319" t="s">
-        <v>496</v>
-      </c>
-      <c r="E319" t="s">
-        <v>682</v>
+        <v>499</v>
       </c>
       <c r="F319" t="b">
         <v>0</v>
       </c>
-      <c r="J319" t="s">
-        <v>681</v>
+      <c r="G319" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="320" spans="1:10">
@@ -10573,22 +10575,22 @@
         <v>675</v>
       </c>
       <c r="B320" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C320" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="D320" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E320" t="s">
-        <v>373</v>
+        <v>692</v>
       </c>
       <c r="F320" t="b">
         <v>0</v>
       </c>
       <c r="J320" t="s">
-        <v>676</v>
+        <v>693</v>
       </c>
     </row>
     <row r="321" spans="1:10">
@@ -10596,19 +10598,19 @@
         <v>675</v>
       </c>
       <c r="B321" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C321" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D321" t="s">
-        <v>532</v>
+        <v>496</v>
       </c>
       <c r="E321" t="s">
-        <v>487</v>
+        <v>373</v>
       </c>
       <c r="J321" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="322" spans="1:10">
@@ -10616,76 +10618,82 @@
         <v>675</v>
       </c>
       <c r="B322" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C322" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D322" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="E322" t="s">
+        <v>682</v>
+      </c>
+      <c r="F322" t="b">
+        <v>0</v>
       </c>
       <c r="J322" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="323" spans="1:10">
       <c r="A323" t="s">
-        <v>692</v>
+        <v>675</v>
       </c>
       <c r="B323" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="C323" t="s">
-        <v>752</v>
+        <v>373</v>
       </c>
       <c r="D323" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="E323" t="s">
-        <v>489</v>
+        <v>373</v>
+      </c>
+      <c r="F323" t="b">
+        <v>0</v>
       </c>
       <c r="J323" t="s">
-        <v>695</v>
+        <v>676</v>
       </c>
     </row>
     <row r="324" spans="1:10">
       <c r="A324" t="s">
-        <v>692</v>
+        <v>675</v>
       </c>
       <c r="B324" t="s">
-        <v>153</v>
+        <v>377</v>
       </c>
       <c r="C324" t="s">
-        <v>703</v>
+        <v>378</v>
       </c>
       <c r="D324" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="E324" t="s">
-        <v>703</v>
+        <v>487</v>
       </c>
       <c r="J324" t="s">
-        <v>701</v>
+        <v>679</v>
       </c>
     </row>
     <row r="325" spans="1:10">
       <c r="A325" t="s">
-        <v>692</v>
+        <v>675</v>
       </c>
       <c r="B325" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="C325" t="s">
-        <v>754</v>
+        <v>380</v>
       </c>
       <c r="D325" t="s">
-        <v>496</v>
-      </c>
-      <c r="E325" t="s">
-        <v>661</v>
+        <v>491</v>
       </c>
       <c r="J325" t="s">
-        <v>705</v>
+        <v>680</v>
       </c>
     </row>
     <row r="326" spans="1:10">
@@ -10693,16 +10701,19 @@
         <v>692</v>
       </c>
       <c r="B326" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C326" t="s">
-        <v>776</v>
+        <v>752</v>
       </c>
       <c r="D326" t="s">
-        <v>494</v>
+        <v>496</v>
+      </c>
+      <c r="E326" t="s">
+        <v>489</v>
       </c>
       <c r="J326" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
     </row>
     <row r="327" spans="1:10">
@@ -10710,22 +10721,19 @@
         <v>692</v>
       </c>
       <c r="B327" t="s">
-        <v>391</v>
+        <v>153</v>
       </c>
       <c r="C327" t="s">
-        <v>775</v>
+        <v>703</v>
       </c>
       <c r="D327" t="s">
         <v>496</v>
       </c>
       <c r="E327" t="s">
-        <v>661</v>
-      </c>
-      <c r="F327" t="b">
-        <v>0</v>
+        <v>703</v>
       </c>
       <c r="J327" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="328" spans="1:10">
@@ -10733,19 +10741,19 @@
         <v>692</v>
       </c>
       <c r="B328" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="C328" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D328" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E328" t="s">
-        <v>487</v>
+        <v>661</v>
       </c>
       <c r="J328" t="s">
-        <v>697</v>
+        <v>705</v>
       </c>
     </row>
     <row r="329" spans="1:10">
@@ -10753,16 +10761,16 @@
         <v>692</v>
       </c>
       <c r="B329" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C329" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="D329" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="J329" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="330" spans="1:10">
@@ -10770,16 +10778,22 @@
         <v>692</v>
       </c>
       <c r="B330" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="C330" t="s">
-        <v>728</v>
+        <v>775</v>
       </c>
       <c r="D330" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="E330" t="s">
+        <v>661</v>
+      </c>
+      <c r="F330" t="b">
+        <v>0</v>
       </c>
       <c r="J330" t="s">
-        <v>694</v>
+        <v>700</v>
       </c>
     </row>
     <row r="331" spans="1:10">
@@ -10787,73 +10801,76 @@
         <v>692</v>
       </c>
       <c r="B331" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C331" t="s">
-        <v>433</v>
+        <v>757</v>
       </c>
       <c r="D331" t="s">
-        <v>491</v>
-      </c>
-      <c r="F331" t="b">
-        <v>0</v>
-      </c>
-      <c r="G331" t="b">
-        <v>1</v>
+        <v>532</v>
+      </c>
+      <c r="E331" t="s">
+        <v>487</v>
       </c>
       <c r="J331" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="332" spans="1:10">
       <c r="A332" t="s">
-        <v>13</v>
+        <v>692</v>
       </c>
       <c r="B332" t="s">
-        <v>127</v>
+        <v>389</v>
       </c>
       <c r="C332" t="s">
-        <v>825</v>
+        <v>774</v>
       </c>
       <c r="D332" t="s">
-        <v>532</v>
-      </c>
-      <c r="E332" t="s">
-        <v>487</v>
+        <v>491</v>
+      </c>
+      <c r="J332" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="333" spans="1:10">
       <c r="A333" t="s">
-        <v>13</v>
+        <v>692</v>
       </c>
       <c r="B333" t="s">
-        <v>89</v>
+        <v>383</v>
       </c>
       <c r="C333" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="D333" t="s">
-        <v>495</v>
-      </c>
-      <c r="E333" t="s">
-        <v>616</v>
+        <v>491</v>
+      </c>
+      <c r="J333" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="334" spans="1:10">
       <c r="A334" t="s">
-        <v>13</v>
+        <v>692</v>
       </c>
       <c r="B334" t="s">
-        <v>122</v>
+        <v>384</v>
       </c>
       <c r="C334" t="s">
-        <v>748</v>
+        <v>433</v>
       </c>
       <c r="D334" t="s">
-        <v>496</v>
-      </c>
-      <c r="E334" t="s">
-        <v>616</v>
+        <v>491</v>
+      </c>
+      <c r="F334" t="b">
+        <v>0</v>
+      </c>
+      <c r="G334" t="b">
+        <v>1</v>
+      </c>
+      <c r="J334" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="335" spans="1:10">
@@ -10861,13 +10878,13 @@
         <v>13</v>
       </c>
       <c r="B335" t="s">
-        <v>407</v>
+        <v>127</v>
       </c>
       <c r="C335" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D335" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="E335" t="s">
         <v>487</v>
@@ -10878,290 +10895,284 @@
         <v>13</v>
       </c>
       <c r="B336" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="C336" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D336" t="s">
-        <v>495</v>
+        <v>532</v>
       </c>
       <c r="E336" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="337" spans="1:10">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7">
       <c r="A337" t="s">
         <v>13</v>
       </c>
       <c r="B337" t="s">
-        <v>261</v>
+        <v>122</v>
       </c>
       <c r="C337" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="D337" t="s">
-        <v>532</v>
+        <v>496</v>
       </c>
       <c r="E337" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="338" spans="1:10">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7">
       <c r="A338" t="s">
         <v>13</v>
       </c>
       <c r="B338" t="s">
-        <v>126</v>
+        <v>407</v>
       </c>
       <c r="C338" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D338" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="339" spans="1:10">
+        <v>496</v>
+      </c>
+      <c r="E338" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7">
       <c r="A339" t="s">
         <v>13</v>
       </c>
       <c r="B339" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C339" t="s">
-        <v>85</v>
+        <v>733</v>
       </c>
       <c r="D339" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="340" spans="1:10">
+        <v>532</v>
+      </c>
+      <c r="E339" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7">
       <c r="A340" t="s">
         <v>13</v>
       </c>
       <c r="B340" t="s">
-        <v>114</v>
+        <v>261</v>
       </c>
       <c r="C340" t="s">
-        <v>115</v>
+        <v>745</v>
       </c>
       <c r="D340" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="E340" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="341" spans="1:10">
+    <row r="341" spans="1:7">
       <c r="A341" t="s">
         <v>13</v>
       </c>
       <c r="B341" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C341" t="s">
-        <v>121</v>
+        <v>827</v>
       </c>
       <c r="D341" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="342" spans="1:10">
+    <row r="342" spans="1:7">
       <c r="A342" t="s">
         <v>13</v>
       </c>
       <c r="B342" t="s">
-        <v>250</v>
+        <v>84</v>
       </c>
       <c r="C342" t="s">
-        <v>251</v>
+        <v>85</v>
       </c>
       <c r="D342" t="s">
         <v>491</v>
       </c>
-      <c r="F342" t="b">
-        <v>0</v>
-      </c>
-      <c r="G342" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="343" spans="1:10">
+    </row>
+    <row r="343" spans="1:7">
       <c r="A343" t="s">
         <v>13</v>
       </c>
       <c r="B343" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C343" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D343" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="344" spans="1:10">
+        <v>496</v>
+      </c>
+      <c r="E343" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7">
       <c r="A344" t="s">
         <v>13</v>
       </c>
       <c r="B344" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="C344" t="s">
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="D344" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="345" spans="1:10">
+    <row r="345" spans="1:7">
       <c r="A345" t="s">
         <v>13</v>
       </c>
       <c r="B345" t="s">
-        <v>65</v>
+        <v>250</v>
       </c>
       <c r="C345" t="s">
-        <v>66</v>
+        <v>251</v>
       </c>
       <c r="D345" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="346" spans="1:10">
+        <v>491</v>
+      </c>
+      <c r="F345" t="b">
+        <v>0</v>
+      </c>
+      <c r="G345" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7">
       <c r="A346" t="s">
         <v>13</v>
       </c>
       <c r="B346" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="C346" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="D346" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="347" spans="1:10">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7">
       <c r="A347" t="s">
         <v>13</v>
       </c>
       <c r="B347" t="s">
+        <v>69</v>
+      </c>
+      <c r="C347" t="s">
+        <v>70</v>
+      </c>
+      <c r="D347" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7">
+      <c r="A348" t="s">
+        <v>13</v>
+      </c>
+      <c r="B348" t="s">
+        <v>65</v>
+      </c>
+      <c r="C348" t="s">
+        <v>66</v>
+      </c>
+      <c r="D348" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7">
+      <c r="A349" t="s">
+        <v>13</v>
+      </c>
+      <c r="B349" t="s">
+        <v>67</v>
+      </c>
+      <c r="C349" t="s">
+        <v>68</v>
+      </c>
+      <c r="D349" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7">
+      <c r="A350" t="s">
+        <v>13</v>
+      </c>
+      <c r="B350" t="s">
         <v>254</v>
       </c>
-      <c r="C347" t="s">
+      <c r="C350" t="s">
         <v>255</v>
       </c>
-      <c r="D347" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="348" spans="1:10">
-      <c r="A348" t="s">
+      <c r="D350" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7">
+      <c r="A351" t="s">
         <v>720</v>
       </c>
-      <c r="B348" t="s">
+      <c r="B351" t="s">
         <v>345</v>
       </c>
-      <c r="C348" t="s">
+      <c r="C351" t="s">
         <v>346</v>
       </c>
-      <c r="D348" t="s">
+      <c r="D351" t="s">
         <v>532</v>
       </c>
-      <c r="E348" t="s">
+      <c r="E351" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="349" spans="1:10">
-      <c r="A349" t="s">
+    <row r="352" spans="1:7">
+      <c r="A352" t="s">
         <v>720</v>
       </c>
-      <c r="C349" t="s">
+      <c r="C352" t="s">
         <v>728</v>
       </c>
-      <c r="D349" t="s">
+      <c r="D352" t="s">
         <v>499</v>
       </c>
-      <c r="F349" t="b">
+      <c r="F352" t="b">
         <v>0</v>
       </c>
-      <c r="G349" t="b">
+      <c r="G352" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="350" spans="1:10">
-      <c r="A350" t="s">
-        <v>720</v>
-      </c>
-      <c r="B350" t="s">
-        <v>340</v>
-      </c>
-      <c r="C350" t="s">
-        <v>341</v>
-      </c>
-      <c r="D350" t="s">
-        <v>496</v>
-      </c>
-      <c r="E350" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="351" spans="1:10">
-      <c r="A351" t="s">
-        <v>15</v>
-      </c>
-      <c r="B351" t="s">
-        <v>89</v>
-      </c>
-      <c r="C351" t="s">
-        <v>732</v>
-      </c>
-      <c r="D351" t="s">
-        <v>496</v>
-      </c>
-      <c r="E351" t="s">
-        <v>616</v>
-      </c>
-      <c r="J351" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="352" spans="1:10">
-      <c r="A352" t="s">
-        <v>15</v>
-      </c>
-      <c r="B352" t="s">
-        <v>320</v>
-      </c>
-      <c r="C352" t="s">
-        <v>629</v>
-      </c>
-      <c r="D352" t="s">
-        <v>496</v>
-      </c>
-      <c r="E352" t="s">
-        <v>629</v>
-      </c>
-      <c r="J352" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="353" spans="1:10">
       <c r="A353" t="s">
-        <v>15</v>
+        <v>720</v>
       </c>
       <c r="B353" t="s">
-        <v>88</v>
+        <v>340</v>
       </c>
       <c r="C353" t="s">
-        <v>767</v>
+        <v>341</v>
       </c>
       <c r="D353" t="s">
-        <v>491</v>
-      </c>
-      <c r="J353" t="s">
-        <v>614</v>
+        <v>496</v>
+      </c>
+      <c r="E353" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="354" spans="1:10">
@@ -11169,19 +11180,19 @@
         <v>15</v>
       </c>
       <c r="B354" t="s">
-        <v>284</v>
+        <v>89</v>
       </c>
       <c r="C354" t="s">
-        <v>746</v>
+        <v>732</v>
       </c>
       <c r="D354" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E354" t="s">
-        <v>489</v>
+        <v>616</v>
       </c>
       <c r="J354" t="s">
-        <v>605</v>
+        <v>615</v>
       </c>
     </row>
     <row r="355" spans="1:10">
@@ -11189,22 +11200,19 @@
         <v>15</v>
       </c>
       <c r="B355" t="s">
-        <v>134</v>
+        <v>320</v>
       </c>
       <c r="C355" t="s">
-        <v>768</v>
+        <v>629</v>
       </c>
       <c r="D355" t="s">
         <v>496</v>
       </c>
       <c r="E355" t="s">
-        <v>487</v>
-      </c>
-      <c r="F355" t="b">
-        <v>0</v>
+        <v>629</v>
       </c>
       <c r="J355" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
     </row>
     <row r="356" spans="1:10">
@@ -11212,16 +11220,16 @@
         <v>15</v>
       </c>
       <c r="B356" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="C356" t="s">
-        <v>133</v>
+        <v>767</v>
       </c>
       <c r="D356" t="s">
         <v>491</v>
       </c>
       <c r="J356" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
     </row>
     <row r="357" spans="1:10">
@@ -11229,19 +11237,19 @@
         <v>15</v>
       </c>
       <c r="B357" t="s">
-        <v>371</v>
+        <v>284</v>
       </c>
       <c r="C357" t="s">
-        <v>769</v>
+        <v>746</v>
       </c>
       <c r="D357" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="E357" t="s">
-        <v>675</v>
+        <v>489</v>
       </c>
       <c r="J357" t="s">
-        <v>674</v>
+        <v>605</v>
       </c>
     </row>
     <row r="358" spans="1:10">
@@ -11249,19 +11257,22 @@
         <v>15</v>
       </c>
       <c r="B358" t="s">
-        <v>271</v>
+        <v>134</v>
       </c>
       <c r="C358" t="s">
-        <v>741</v>
+        <v>768</v>
       </c>
       <c r="D358" t="s">
-        <v>532</v>
+        <v>496</v>
       </c>
       <c r="E358" t="s">
-        <v>489</v>
+        <v>487</v>
+      </c>
+      <c r="F358" t="b">
+        <v>0</v>
       </c>
       <c r="J358" t="s">
-        <v>603</v>
+        <v>624</v>
       </c>
     </row>
     <row r="359" spans="1:10">
@@ -11269,16 +11280,16 @@
         <v>15</v>
       </c>
       <c r="B359" t="s">
-        <v>288</v>
+        <v>132</v>
       </c>
       <c r="C359" t="s">
-        <v>770</v>
+        <v>133</v>
       </c>
       <c r="D359" t="s">
         <v>491</v>
       </c>
       <c r="J359" t="s">
-        <v>610</v>
+        <v>623</v>
       </c>
     </row>
     <row r="360" spans="1:10">
@@ -11286,22 +11297,19 @@
         <v>15</v>
       </c>
       <c r="B360" t="s">
-        <v>141</v>
+        <v>371</v>
       </c>
       <c r="C360" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D360" t="s">
-        <v>532</v>
+        <v>496</v>
       </c>
       <c r="E360" t="s">
-        <v>502</v>
-      </c>
-      <c r="F360" t="b">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="J360" t="s">
-        <v>598</v>
+        <v>674</v>
       </c>
     </row>
     <row r="361" spans="1:10">
@@ -11309,16 +11317,19 @@
         <v>15</v>
       </c>
       <c r="B361" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C361" t="s">
-        <v>283</v>
+        <v>741</v>
       </c>
       <c r="D361" t="s">
-        <v>491</v>
+        <v>532</v>
+      </c>
+      <c r="E361" t="s">
+        <v>489</v>
       </c>
       <c r="J361" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="362" spans="1:10">
@@ -11326,16 +11337,16 @@
         <v>15</v>
       </c>
       <c r="B362" t="s">
-        <v>86</v>
+        <v>288</v>
       </c>
       <c r="C362" t="s">
-        <v>87</v>
+        <v>770</v>
       </c>
       <c r="D362" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J362" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="363" spans="1:10">
@@ -11343,13 +11354,13 @@
         <v>15</v>
       </c>
       <c r="B363" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C363" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D363" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="E363" t="s">
         <v>502</v>
@@ -11358,7 +11369,7 @@
         <v>0</v>
       </c>
       <c r="J363" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="364" spans="1:10">
@@ -11366,19 +11377,16 @@
         <v>15</v>
       </c>
       <c r="B364" t="s">
-        <v>82</v>
+        <v>282</v>
       </c>
       <c r="C364" t="s">
-        <v>773</v>
+        <v>283</v>
       </c>
       <c r="D364" t="s">
-        <v>495</v>
-      </c>
-      <c r="E364" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="J364" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
     </row>
     <row r="365" spans="1:10">
@@ -11386,16 +11394,16 @@
         <v>15</v>
       </c>
       <c r="B365" t="s">
-        <v>286</v>
+        <v>86</v>
       </c>
       <c r="C365" t="s">
-        <v>287</v>
+        <v>87</v>
       </c>
       <c r="D365" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="J365" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="366" spans="1:10">
@@ -11403,16 +11411,22 @@
         <v>15</v>
       </c>
       <c r="B366" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="C366" t="s">
-        <v>85</v>
+        <v>772</v>
       </c>
       <c r="D366" t="s">
-        <v>491</v>
+        <v>496</v>
+      </c>
+      <c r="E366" t="s">
+        <v>502</v>
+      </c>
+      <c r="F366" t="b">
+        <v>0</v>
       </c>
       <c r="J366" t="s">
-        <v>612</v>
+        <v>597</v>
       </c>
     </row>
     <row r="367" spans="1:10">
@@ -11420,16 +11434,19 @@
         <v>15</v>
       </c>
       <c r="B367" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C367" t="s">
-        <v>81</v>
+        <v>773</v>
       </c>
       <c r="D367" t="s">
-        <v>494</v>
+        <v>532</v>
+      </c>
+      <c r="E367" t="s">
+        <v>487</v>
       </c>
       <c r="J367" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="368" spans="1:10">
@@ -11437,16 +11454,16 @@
         <v>15</v>
       </c>
       <c r="B368" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="C368" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="D368" t="s">
         <v>491</v>
       </c>
       <c r="J368" t="s">
-        <v>625</v>
+        <v>609</v>
       </c>
     </row>
     <row r="369" spans="1:10">
@@ -11454,16 +11471,16 @@
         <v>15</v>
       </c>
       <c r="B369" t="s">
-        <v>280</v>
+        <v>84</v>
       </c>
       <c r="C369" t="s">
-        <v>281</v>
+        <v>85</v>
       </c>
       <c r="D369" t="s">
         <v>491</v>
       </c>
       <c r="J369" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
     </row>
     <row r="370" spans="1:10">
@@ -11471,16 +11488,16 @@
         <v>15</v>
       </c>
       <c r="B370" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C370" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D370" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="J370" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="371" spans="1:10">
@@ -11488,19 +11505,16 @@
         <v>15</v>
       </c>
       <c r="B371" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C371" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="D371" t="s">
-        <v>524</v>
-      </c>
-      <c r="H371" t="s">
-        <v>607</v>
+        <v>491</v>
       </c>
       <c r="J371" t="s">
-        <v>608</v>
+        <v>625</v>
       </c>
     </row>
     <row r="372" spans="1:10">
@@ -11508,16 +11522,16 @@
         <v>15</v>
       </c>
       <c r="B372" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="C372" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="D372" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J372" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
     </row>
     <row r="373" spans="1:10">
@@ -11525,16 +11539,16 @@
         <v>15</v>
       </c>
       <c r="B373" t="s">
-        <v>274</v>
+        <v>78</v>
       </c>
       <c r="C373" t="s">
-        <v>275</v>
+        <v>79</v>
       </c>
       <c r="D373" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="J373" t="s">
-        <v>626</v>
+        <v>599</v>
       </c>
     </row>
     <row r="374" spans="1:10">
@@ -11542,16 +11556,19 @@
         <v>15</v>
       </c>
       <c r="B374" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C374" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D374" t="s">
-        <v>492</v>
+        <v>524</v>
+      </c>
+      <c r="H374" t="s">
+        <v>607</v>
       </c>
       <c r="J374" t="s">
-        <v>627</v>
+        <v>608</v>
       </c>
     </row>
     <row r="375" spans="1:10">
@@ -11559,83 +11576,134 @@
         <v>15</v>
       </c>
       <c r="B375" t="s">
-        <v>269</v>
+        <v>292</v>
       </c>
       <c r="C375" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
       <c r="D375" t="s">
-        <v>491</v>
-      </c>
-      <c r="F375" t="b">
-        <v>0</v>
-      </c>
-      <c r="G375" t="b">
-        <v>1</v>
+        <v>494</v>
       </c>
       <c r="J375" t="s">
-        <v>602</v>
+        <v>611</v>
       </c>
     </row>
     <row r="376" spans="1:10">
       <c r="A376" t="s">
-        <v>548</v>
+        <v>15</v>
       </c>
       <c r="B376" t="s">
-        <v>451</v>
+        <v>274</v>
       </c>
       <c r="C376" t="s">
-        <v>452</v>
+        <v>275</v>
       </c>
       <c r="D376" t="s">
-        <v>501</v>
-      </c>
-      <c r="F376" t="b">
-        <v>0</v>
-      </c>
-      <c r="G376" t="b">
-        <v>1</v>
+        <v>498</v>
       </c>
       <c r="J376" t="s">
-        <v>549</v>
+        <v>626</v>
       </c>
     </row>
     <row r="377" spans="1:10">
       <c r="A377" t="s">
-        <v>551</v>
+        <v>15</v>
       </c>
       <c r="B377" t="s">
-        <v>461</v>
+        <v>276</v>
       </c>
       <c r="C377" t="s">
-        <v>462</v>
+        <v>277</v>
       </c>
       <c r="D377" t="s">
-        <v>491</v>
-      </c>
-      <c r="F377" t="b">
-        <v>0</v>
-      </c>
-      <c r="G377" t="b">
-        <v>1</v>
+        <v>492</v>
+      </c>
+      <c r="J377" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="378" spans="1:10">
       <c r="A378" t="s">
+        <v>15</v>
+      </c>
+      <c r="B378" t="s">
+        <v>269</v>
+      </c>
+      <c r="C378" t="s">
+        <v>270</v>
+      </c>
+      <c r="D378" t="s">
+        <v>491</v>
+      </c>
+      <c r="F378" t="b">
+        <v>0</v>
+      </c>
+      <c r="G378" t="b">
+        <v>1</v>
+      </c>
+      <c r="J378" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="379" spans="1:10">
+      <c r="A379" t="s">
+        <v>548</v>
+      </c>
+      <c r="B379" t="s">
+        <v>451</v>
+      </c>
+      <c r="C379" t="s">
+        <v>452</v>
+      </c>
+      <c r="D379" t="s">
+        <v>501</v>
+      </c>
+      <c r="F379" t="b">
+        <v>0</v>
+      </c>
+      <c r="G379" t="b">
+        <v>1</v>
+      </c>
+      <c r="J379" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="380" spans="1:10">
+      <c r="A380" t="s">
         <v>551</v>
       </c>
-      <c r="B378" t="s">
+      <c r="B380" t="s">
+        <v>461</v>
+      </c>
+      <c r="C380" t="s">
+        <v>462</v>
+      </c>
+      <c r="D380" t="s">
+        <v>491</v>
+      </c>
+      <c r="F380" t="b">
+        <v>0</v>
+      </c>
+      <c r="G380" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10">
+      <c r="A381" t="s">
+        <v>551</v>
+      </c>
+      <c r="B381" t="s">
         <v>463</v>
       </c>
-      <c r="C378" t="s">
+      <c r="C381" t="s">
         <v>464</v>
       </c>
-      <c r="D378" t="s">
+      <c r="D381" t="s">
         <v>491</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J378">
+  <autoFilter ref="A1:J381">
     <sortState ref="A2:J378">
       <sortCondition ref="A1:A378"/>
     </sortState>

</xml_diff>

<commit_message>
Add entity tag, update package tags to use new Relation options.
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/DICOM_MODEL.xlsx
+++ b/molgenis-model-registry/src/test/resources/DICOM_MODEL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="920" windowWidth="26020" windowHeight="16680" tabRatio="951" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14420" tabRatio="951" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="25" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="855">
   <si>
     <t>description</t>
   </si>
@@ -2571,9 +2571,6 @@
     <t>NameOfPhysiciansReading</t>
   </si>
   <si>
-    <t>Digital Imaging and Communications in Medicine (DICOM) is the standard for the communication and management of medical imaging information and related data. This is not the full model, but shows the core entities. Website: http://dicom.nema.org . Documentation: http://medical.nema.org/standard.html .</t>
-  </si>
-  <si>
     <t>identifier</t>
   </si>
   <si>
@@ -2586,15 +2583,9 @@
     <t>codeSystem</t>
   </si>
   <si>
-    <t>relationIRI</t>
-  </si>
-  <si>
     <t>system</t>
   </si>
   <si>
-    <t>http://molgenis.org/biobankconnect/link</t>
-  </si>
-  <si>
     <t>dicom_home</t>
   </si>
   <si>
@@ -2610,13 +2601,55 @@
     <t>http://www.biosharing.org/bsg-000114</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
     <t>dicom_biosharing</t>
   </si>
   <si>
-    <t>dicom_home,dicom_biosharing</t>
+    <t>hl7_website</t>
+  </si>
+  <si>
+    <t>http://www.hl7.org/</t>
+  </si>
+  <si>
+    <t>HL7</t>
+  </si>
+  <si>
+    <t>relationIri</t>
+  </si>
+  <si>
+    <t>http://xmlns.com/foaf/0.1/homepage</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/01/rdf-schema#isDefinedBy</t>
+  </si>
+  <si>
+    <t>isDefinedBy</t>
+  </si>
+  <si>
+    <t>homepage</t>
+  </si>
+  <si>
+    <t>dicom_isDefinedBy</t>
+  </si>
+  <si>
+    <t>http://medical.nema.org/standard.html</t>
+  </si>
+  <si>
+    <t>The Dicom Standard</t>
+  </si>
+  <si>
+    <t>Biosharing</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/01/rdf-schema#seeAlso</t>
+  </si>
+  <si>
+    <t>seeAlso</t>
+  </si>
+  <si>
+    <t>Digital Imaging and Communications in Medicine (DICOM) is the standard for the communication and management of medical imaging information and related data. This is not the full model, but shows the core entities.</t>
+  </si>
+  <si>
+    <t>dicom_home,dicom_biosharing,dicom_isDefinedBy</t>
   </si>
 </sst>
 </file>
@@ -2693,7 +2726,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="701">
+  <cellStyleXfs count="717">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3395,13 +3428,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="701">
+  <cellStyles count="717">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3880,6 +3935,14 @@
     <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4102,6 +4165,14 @@
     <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4434,35 +4505,35 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="135.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>828</v>
+      <c r="B2" s="4" t="s">
+        <v>853</v>
       </c>
       <c r="C2" t="s">
-        <v>843</v>
+        <v>854</v>
       </c>
     </row>
   </sheetData>
@@ -4477,20 +4548,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="255.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="51.1640625" style="4" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="20">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="20">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -4500,11 +4571,14 @@
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="2" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>718</v>
       </c>
@@ -4515,7 +4589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -4526,7 +4600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -4537,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>487</v>
       </c>
@@ -4548,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>682</v>
       </c>
@@ -4559,7 +4633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>373</v>
       </c>
@@ -4570,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>661</v>
       </c>
@@ -4581,7 +4655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>545</v>
       </c>
@@ -4592,7 +4666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>541</v>
       </c>
@@ -4603,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>240</v>
       </c>
@@ -4614,7 +4688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>719</v>
       </c>
@@ -4625,7 +4699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>489</v>
       </c>
@@ -4635,8 +4709,11 @@
       <c r="C13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>712</v>
       </c>
@@ -4647,7 +4724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>708</v>
       </c>
@@ -4658,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -4702,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="45">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -4712,7 +4789,7 @@
       <c r="C20" t="b">
         <v>0</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4738,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="90">
       <c r="A23" t="s">
         <v>726</v>
       </c>
@@ -4748,7 +4825,7 @@
       <c r="C23" t="b">
         <v>0</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4928,7 +5005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" ht="45">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -4938,7 +5015,7 @@
       <c r="C40" t="b">
         <v>0</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4975,7 +5052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" ht="90">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -4985,7 +5062,7 @@
       <c r="C44" t="b">
         <v>0</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5000,7 +5077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" ht="120">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -5010,7 +5087,7 @@
       <c r="C46" t="b">
         <v>0</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5051,9 +5128,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J381"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G319" sqref="G319"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11721,9 +11798,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -11732,67 +11809,107 @@
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="33.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>829</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>830</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>831</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>832</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>838</v>
+      </c>
+      <c r="B4" t="s">
         <v>837</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>838</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>834</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>842</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
+        <v>850</v>
+      </c>
+      <c r="D4" t="s">
+        <v>852</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="F4" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>839</v>
+      </c>
+      <c r="B5" t="s">
         <v>840</v>
       </c>
-      <c r="C3" t="s">
-        <v>840</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C5" t="s">
         <v>841</v>
       </c>
-      <c r="E3" t="s">
-        <v>834</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>835</v>
+      <c r="D5" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="F5" t="s">
+        <v>832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>